<commit_message>
added list of features in checklist_customization.xlsx file
</commit_message>
<xml_diff>
--- a/check list customization.xlsx
+++ b/check list customization.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="features" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Mandatory Field to be displayed based on condition</t>
   </si>
@@ -97,6 +98,129 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>1. Introduction to Frappe framework and the ERPNext application</t>
+  </si>
+  <si>
+    <t>2. Installation of Frappe Framework</t>
+  </si>
+  <si>
+    <t>3. Creatingasite to work with ERPNext</t>
+  </si>
+  <si>
+    <t>4. Installing ERPNext onasite</t>
+  </si>
+  <si>
+    <t>5. Frappe Field Types</t>
+  </si>
+  <si>
+    <t>6. Introduction to the frappe desk</t>
+  </si>
+  <si>
+    <t>7. Creatingacustom app</t>
+  </si>
+  <si>
+    <t>8. Installing the custom app on your site</t>
+  </si>
+  <si>
+    <t>9. Exploring the Frappe DocTypes</t>
+  </si>
+  <si>
+    <t>10. Working with Dependent Fields</t>
+  </si>
+  <si>
+    <t>11. Introduction to Custom Scripts</t>
+  </si>
+  <si>
+    <t>12. Using Custom Scripts to make API Calls</t>
+  </si>
+  <si>
+    <t>13. Using Custom Scripts to do Arithmetics</t>
+  </si>
+  <si>
+    <t>14. Working with Server Scripts</t>
+  </si>
+  <si>
+    <t>15. Working with Menus in Custom Applications</t>
+  </si>
+  <si>
+    <t>16. Email Functionality</t>
+  </si>
+  <si>
+    <t>17. Creating custom reports</t>
+  </si>
+  <si>
+    <t>18. Customizing the print format</t>
+  </si>
+  <si>
+    <t>19. Working with schedulers</t>
+  </si>
+  <si>
+    <t>20. Introduction to the Frappe Dialog API</t>
+  </si>
+  <si>
+    <t>21. URL Routing</t>
+  </si>
+  <si>
+    <t>22. Working with Currencies</t>
+  </si>
+  <si>
+    <t>23. Implementing content pagination</t>
+  </si>
+  <si>
+    <t>24. Exploring the Frappe Chart</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>1. Working with Controllers, ORM and SQL in Frappe Framework</t>
+  </si>
+  <si>
+    <t>2. Hooks and DocType manipulation from events</t>
+  </si>
+  <si>
+    <t>3. ERPNext integration with devices (We will integrateabiometric device)</t>
+  </si>
+  <si>
+    <t>4. Writing custom APIS within the ERPNext ecosystem</t>
+  </si>
+  <si>
+    <t>5. Consuming custom APIS from other software applications</t>
+  </si>
+  <si>
+    <t>6. Sending data from ERPNext to other applications with Web Hooks</t>
+  </si>
+  <si>
+    <t>7. Using Events to manipulate Doctypes</t>
+  </si>
+  <si>
+    <t>8. Building web apps in Frappe Framework</t>
+  </si>
+  <si>
+    <t>9. Working withabootstrap template on Frappe Framework</t>
+  </si>
+  <si>
+    <t>10. Working with dynamic data on the custom web app</t>
+  </si>
+  <si>
+    <t>11. Error Handling in Frappe Framework</t>
+  </si>
+  <si>
+    <t>12. Building custom pages in Frappe Framework</t>
+  </si>
+  <si>
+    <t>13. Managing your ERPNext instance and custom apps with GitHub</t>
+  </si>
+  <si>
+    <t>14. Setting up Frappe for multi-tenancy</t>
+  </si>
+  <si>
+    <t>15. ERPNext for E-Commerce</t>
   </si>
 </sst>
 </file>
@@ -460,7 +584,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,4 +729,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>